<commit_message>
new art + reloader
</commit_message>
<xml_diff>
--- a/public/dist/expositions.xlsx
+++ b/public/dist/expositions.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>Nom</t>
   </si>
@@ -51,55 +51,6 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Traces &amp; Empreintes</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>,La Vieille Forge, Saint Paul, avec 2 invités Philippe Bellissent et Chantal Dachez. Du 17 au 30 mai 2014.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Les Voiles d'Antibes</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>, 4-8 Juin,le grand rdv du yachting de tradition: j'y expose mes bleus,esplanade du chantier naval Opéra, Port Vauban, proche du Quai des Milliardaires.</t>
-    </r>
-  </si>
-  <si>
-    <t>Couleurs de Printemps, Saint Paul de Vence, La Vieille Forge. Avril 2014</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
       <t>Le Carré au Cercle</t>
     </r>
     <r>
@@ -179,25 +130,10 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Expo "Malins Plaisirs", avril-mai 2013, Galerie des Dominicains, Vieux Nice. </t>
-  </si>
-  <si>
     <t>Oui</t>
   </si>
   <si>
     <t>https://www.google.ca/maps/place/Galerie+des+Dominicains/@43.695834,7.271766,17z/data=!3m1!4b1!4m2!3m1!1s0x0:0x8724e442bfa2669b</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Démarche : </t>
-  </si>
-  <si>
-    <t>Raconter une histoire, un petit rien ou un paysage imaginaire. Aspérités des grains de sable, assemblages de textures et de formes, collages, éraflures, marques, traces, écritures...je fais et défais, enlève et rajoute, à la recherche de textures qui vibrent et d'une poésie qui ne doit rien à la technique.</t>
-  </si>
-  <si>
-    <t>Telling a story, a sliver of nothing or an imaginary one. Done with grains of sand, texture and form, collages, marks and traces and writing. A reconstruction to touch with sight. Welcome to my colors of uplifting art!</t>
-  </si>
-  <si>
-    <t>Statement :</t>
   </si>
   <si>
     <t>Washington DC, USA, Octobre04 : organise et participe à "14 Ways", exposition prestigieuse à l'Ambassade de France aux USA. Group exhibit at the Embassy of France, Washington , DC.</t>
@@ -305,6 +241,133 @@
   </si>
   <si>
     <r>
+      <t xml:space="preserve">Démarche/ </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="12"/>
+        <color theme="4" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Statement</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="4" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> :</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Raconter une histoire, un petit rien ou un paysage imaginaire. Aspérités des grains de sable, assemblages de textures et de formes, collages, éraflures, marques, traces, écritures...je fais et défais, enlève et rajoute, à la recherche de textures qui vibrent et d'une poésie qui ne doit rien à la technique./ </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="4" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Telling a story, a sliver of nothing or an imaginary one. Done with grains of sand, texture and form, collages, marks and traces and writing. A reconstruction to touch with sight. Welcome to my colors of uplifting art!</t>
+    </r>
+  </si>
+  <si>
+    <t>expositions récentes / last exhibits</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Expo solo</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "Malins Plaisirs", avril-mai 2013, Galerie des Dominicains, Vieux Nice. </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Les Voiles d'Antibes</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, 4-8 Juin,le grand rdv du yachting de tradition, blue exhibition.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Traces &amp; Empreintes</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>,La Vieille Forge, Saint Paul, avec 2 invités Phil Bellissent et Ch Dachez, mai 2014.</t>
+    </r>
+  </si>
+  <si>
+    <r>
       <rPr>
         <sz val="12"/>
         <color theme="1"/>
@@ -335,8 +398,8 @@
         <scheme val="minor"/>
       </rPr>
       <t>ernissage le samedi 5 juillet à 19h à la Vieille Forge, Place du Tilleul
-Le corps n'a cessé d'interroger les Artistes qui y ont trouvé une source inépuisable d'inspirations. C’est à cette inspiration que se nourrissent les Artistes du Cercle en cet été 2014 pour animer la vieille forge, place du tilleul avec un format unique de kakémono
-La Vieille Forge, place du Tilleul, Saint-Paul de Vence. Ouverture tous les jours de 15h à 19h, jusqu'au 31 aout2014.   http://www.cercledesartistesdesaintpauldevence.com/
+Le corps n'a cessé d'interroger les Artistes qui y ont trouvé une source inépuisable d'inspirations. C’est à cette inspiration que se nourrissent les Artistes du Cercle en cet été 2014 pour animer la vieille forge, place du tilleul. Format unique de kakémono en 150x70cm. 
+Tous les jours de 15h à 19h, jusque fin aout2014.   http://www.cercledesartistesdesaintpauldevence.com/
 https://www.facebook.com/casp.saintpaul</t>
     </r>
   </si>
@@ -345,7 +408,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+  <fonts count="8">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -377,6 +440,39 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="12"/>
+      <color theme="4" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="4" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color theme="4" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="9" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -399,7 +495,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -409,6 +505,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -743,10 +842,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
@@ -780,28 +879,28 @@
     </row>
     <row r="2" spans="1:6" ht="110.25">
       <c r="A2" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="C2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="94.5">
+      <c r="A3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="110.25">
-      <c r="A3" s="1" t="s">
+      <c r="B3" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>25</v>
-      </c>
       <c r="D3" s="3"/>
     </row>
-    <row r="4" spans="1:6" ht="31.5">
+    <row r="4" spans="1:6" ht="63">
       <c r="A4" s="1" t="s">
         <v>17</v>
       </c>
@@ -810,18 +909,16 @@
       </c>
       <c r="D4" s="3"/>
     </row>
-    <row r="5" spans="1:6" ht="31.5">
-      <c r="A5" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B5" s="4" t="s">
+    <row r="5" spans="1:6">
+      <c r="A5" s="1"/>
+      <c r="B5" s="5" t="s">
         <v>19</v>
       </c>
       <c r="D5" s="3"/>
     </row>
     <row r="6" spans="1:6">
       <c r="B6" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="C6" t="s">
         <v>6</v>
@@ -829,42 +926,37 @@
     </row>
     <row r="7" spans="1:6">
       <c r="B7" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="B8" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="B9" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="B10" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="B11" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="B12" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="B13" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6">
-      <c r="B14" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>